<commit_message>
making the spreads logic into a function
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week7.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week7.xlsx
@@ -516,40 +516,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>San Diego State</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3.7</v>
+        <v>2.6</v>
       </c>
       <c r="E2" t="n">
-        <v>5.800000000000001</v>
+        <v>6.199999999999999</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>San Diego State -7.0</t>
+          <t>Jacksonville State -9.0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>San Diego State -6.5</t>
+          <t>Jacksonville State -7.5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>San Diego State -12.3</t>
+          <t>Jacksonville State -13.7</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>-12.3</v>
+        <v>-13.7</v>
       </c>
       <c r="J2" t="n">
-        <v>-6.5</v>
+        <v>-7.5</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -566,40 +566,40 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>UL Monroe</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2.6</v>
+        <v>4.8</v>
       </c>
       <c r="E3" t="n">
-        <v>5.199999999999999</v>
+        <v>4.9</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Jacksonville State -8.5</t>
+          <t>UL Monroe -2.5</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Jacksonville State -8.5</t>
+          <t>UL Monroe -3.0</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Jacksonville State -13.7</t>
+          <t>Coastal Carolina -1.9</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>-13.7</v>
+        <v>1.9</v>
       </c>
       <c r="J3" t="n">
-        <v>-8.5</v>
+        <v>-3</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -616,40 +616,40 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>San Diego State</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.1</v>
+        <v>3.7</v>
       </c>
       <c r="E4" t="n">
-        <v>4.699999999999999</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Louisiana Tech -5.5</t>
+          <t>San Diego State -6.5</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Louisiana Tech -6.5</t>
+          <t>San Diego State -7.5</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Louisiana Tech -11.2</t>
+          <t>San Diego State -12.3</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>-11.2</v>
+        <v>-12.3</v>
       </c>
       <c r="J4" t="n">
-        <v>-6.5</v>
+        <v>-7.5</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -666,40 +666,40 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>9.800000000000001</v>
+        <v>4.1</v>
       </c>
       <c r="E5" t="n">
-        <v>4.6</v>
+        <v>4.699999999999999</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Texas -9.5</t>
+          <t>Louisiana Tech -6.5</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Texas -3</t>
+          <t>Louisiana Tech -6.5</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Oklahoma -1.6</t>
+          <t>Louisiana Tech -11.2</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>-1.6</v>
+        <v>-11.2</v>
       </c>
       <c r="J5" t="n">
-        <v>3</v>
+        <v>-6.5</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -716,40 +716,40 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Air Force</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="E6" t="n">
-        <v>4.6</v>
+        <v>4.1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Toledo -7.0</t>
+          <t>UNLV -7.0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Toledo -9.5</t>
+          <t>UNLV -6.0</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Toledo -14.1</t>
+          <t>UNLV -10.1</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>-14.1</v>
+        <v>10.1</v>
       </c>
       <c r="J6" t="n">
-        <v>-9.5</v>
+        <v>6</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -766,40 +766,40 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>UL Monroe</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4.8</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>4.4</v>
+        <v>3.9</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>UL Monroe -2.5</t>
+          <t>Tulane -7.0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>UL Monroe -2.5</t>
+          <t>Tulane -6.5</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Coastal Carolina -1.9</t>
+          <t>Tulane -2.6</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1.9</v>
+        <v>2.6</v>
       </c>
       <c r="J7" t="n">
-        <v>-2.5</v>
+        <v>6.5</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -816,40 +816,40 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8.800000000000001</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>4.4</v>
+        <v>3.8</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Tulane -7.0</t>
+          <t>Florida State -9.5</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Tulane -7</t>
+          <t>Florida State -10.5</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Tulane -2.6</t>
+          <t>Florida State -6.7</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2.6</v>
+        <v>6.7</v>
       </c>
       <c r="J8" t="n">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
@@ -882,7 +882,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Hawai'i -1.5</t>
+          <t>Hawai'i -2.0</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -916,40 +916,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Army</t>
+          <t>North Texas</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="D10" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>North Texas -1.5</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>South Florida -1.0</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>North Texas -2.7</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
         <v>2.7</v>
       </c>
-      <c r="E10" t="n">
-        <v>3.699999999999999</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Army -20.5</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Army -17.5</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Army -21.2</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>21.2</v>
-      </c>
       <c r="J10" t="n">
-        <v>17.5</v>
+        <v>-1</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -966,40 +966,40 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Army</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Arizona State</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>9.199999999999999</v>
+        <v>2.7</v>
       </c>
       <c r="E11" t="n">
-        <v>3.6</v>
+        <v>3.699999999999999</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Utah -2.5</t>
+          <t>Army -17.5</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Utah -5.5</t>
+          <t>Army -17.5</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Utah -9.1</t>
+          <t>Army -21.2</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>9.1</v>
+        <v>21.2</v>
       </c>
       <c r="J11" t="n">
-        <v>5.5</v>
+        <v>17.5</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -1016,40 +1016,40 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Air Force</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="E12" t="n">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>UNLV -7.0</t>
+          <t>Toledo -8.5</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>UNLV -7</t>
+          <t>Toledo -10.5</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>UNLV -10.1</t>
+          <t>Toledo -14.1</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>10.1</v>
+        <v>-14.1</v>
       </c>
       <c r="J12" t="n">
-        <v>7</v>
+        <v>-10.5</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -1066,40 +1066,40 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Michigan State</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>7.1</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Michigan State -8.5</t>
+          <t>TCU -1.5</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Michigan State -7.5</t>
+          <t>TCU -1.0</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Michigan State -10.5</t>
+          <t>TCU -4.3</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>10.5</v>
+        <v>-4.3</v>
       </c>
       <c r="J13" t="n">
-        <v>7.5</v>
+        <v>-1</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
@@ -1116,40 +1116,40 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>BYU</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>9.300000000000001</v>
+        <v>8.9</v>
       </c>
       <c r="E14" t="n">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Florida State -8.5</t>
+          <t>BYU -2.5</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Florida State -9.5</t>
+          <t>BYU -1.5</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Florida State -6.7</t>
+          <t>BYU -4.7</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>6.7</v>
+        <v>-4.7</v>
       </c>
       <c r="J14" t="n">
-        <v>9.5</v>
+        <v>-1.5</v>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
@@ -1166,40 +1166,40 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8.699999999999999</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>TCU -2.5</t>
+          <t>Texas -3.0</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>TCU -1.5</t>
+          <t>Texas -1.5</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>TCU -4.3</t>
+          <t>Oklahoma -1.6</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>-4.3</v>
+        <v>-1.6</v>
       </c>
       <c r="J15" t="n">
-        <v>-1.5</v>
+        <v>1.5</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
@@ -1216,40 +1216,40 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>Arizona State</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>6.2</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>San José State -1.5</t>
+          <t>Utah -5.5</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>San José State -2.5</t>
+          <t>Utah -6.0</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Wyoming -0.2</t>
+          <t>Utah -9.1</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0.2</v>
+        <v>9.1</v>
       </c>
       <c r="J16" t="n">
-        <v>-2.5</v>
+        <v>6</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -1266,40 +1266,40 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>6.4</v>
+        <v>4.1</v>
       </c>
       <c r="E17" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Clemson -12.5</t>
+          <t>Western Michigan -9.5</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Clemson -14</t>
+          <t>Western Michigan -8.5</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Clemson -11.5</t>
+          <t>Western Michigan -11.5</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>-11.5</v>
+        <v>11.5</v>
       </c>
       <c r="J17" t="n">
-        <v>-14</v>
+        <v>8.5</v>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
@@ -1316,40 +1316,40 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Troy</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>6.7</v>
+        <v>6.4</v>
       </c>
       <c r="E18" t="n">
-        <v>2.300000000000001</v>
+        <v>3</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Texas State -10.0</t>
+          <t>Clemson -13.5</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Texas State -10.5</t>
+          <t>Clemson -14.5</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Texas State -8.2</t>
+          <t>Clemson -11.5</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>8.199999999999999</v>
+        <v>-11.5</v>
       </c>
       <c r="J18" t="n">
-        <v>10.5</v>
+        <v>-14.5</v>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
@@ -1366,40 +1366,40 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>UAB</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>5.1</v>
+        <v>3.3</v>
       </c>
       <c r="E19" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Florida Atlantic -4.5</t>
+          <t>Missouri State -3.0</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Florida Atlantic -4.5</t>
+          <t>Missouri State -2.0</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Florida Atlantic -6.8</t>
+          <t>Missouri State -4.5</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>6.8</v>
+        <v>-4.5</v>
       </c>
       <c r="J19" t="n">
-        <v>4.5</v>
+        <v>-2</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1416,40 +1416,40 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BYU</t>
+          <t>UAB</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>8.9</v>
+        <v>5.1</v>
       </c>
       <c r="E20" t="n">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>BYU -3.0</t>
+          <t>Florida Atlantic -5.5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>BYU -2.5</t>
+          <t>Florida Atlantic -4.5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>BYU -4.7</t>
+          <t>Florida Atlantic -6.8</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>-4.7</v>
+        <v>6.8</v>
       </c>
       <c r="J20" t="n">
-        <v>-2.5</v>
+        <v>4.5</v>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
@@ -1466,40 +1466,40 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="E21" t="n">
         <v>2.199999999999999</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Ohio State -13.5</t>
+          <t>LSU -10.0</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Ohio State -15.5</t>
+          <t>LSU -8.5</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Ohio State -13.3</t>
+          <t>LSU -10.7</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>-13.3</v>
+        <v>10.7</v>
       </c>
       <c r="J21" t="n">
-        <v>-15.5</v>
+        <v>8.5</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
@@ -1566,40 +1566,40 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>Northern Illinois</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.1</v>
+        <v>4</v>
       </c>
       <c r="E23" t="n">
         <v>2</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Western Michigan -10.0</t>
+          <t>Eastern Michigan -1.0</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Western Michigan -9.5</t>
+          <t>Northern Illinois -1.5</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Western Michigan -11.5</t>
+          <t>Northern Illinois -3.5</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>11.5</v>
+        <v>-3.5</v>
       </c>
       <c r="J23" t="n">
-        <v>9.5</v>
+        <v>-1.5</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
@@ -1616,40 +1616,40 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Northern Illinois</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4</v>
+        <v>4.6</v>
       </c>
       <c r="E24" t="n">
         <v>2</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Eastern Michigan -1.5</t>
+          <t>Fresno State -6.5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Northern Illinois -1.5</t>
+          <t>Fresno State -6.5</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Northern Illinois -3.5</t>
+          <t>Fresno State -8.5</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>-3.5</v>
+        <v>-8.5</v>
       </c>
       <c r="J24" t="n">
-        <v>-1.5</v>
+        <v>-6.5</v>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
@@ -1666,40 +1666,40 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.3</v>
+        <v>7.3</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Missouri State -3.5</t>
+          <t>Minnesota -10.0</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Missouri State -2.5</t>
+          <t>Minnesota -8.0</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Missouri State -4.5</t>
+          <t>Minnesota -9.9</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>-4.5</v>
+        <v>9.9</v>
       </c>
       <c r="J25" t="n">
-        <v>-2.5</v>
+        <v>8</v>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
@@ -1716,40 +1716,40 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.6</v>
+        <v>9.4</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Fresno State -7.0</t>
+          <t>Texas A&amp;M -7.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Fresno State -6.5</t>
+          <t>Texas A&amp;M -7.5</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Fresno State -8.5</t>
+          <t>Texas A&amp;M -9.3</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>-8.5</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="J26" t="n">
-        <v>-6.5</v>
+        <v>7.5</v>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
@@ -1766,40 +1766,40 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>6.3</v>
+        <v>4.9</v>
       </c>
       <c r="E27" t="n">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Boise State -16.5</t>
+          <t>Liberty -2.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Boise State -16.5</t>
+          <t>Liberty -1.0</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Boise State -14.6</t>
+          <t>Liberty -2.7</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>14.6</v>
+        <v>-2.7</v>
       </c>
       <c r="J27" t="n">
-        <v>16.5</v>
+        <v>-1</v>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
@@ -1816,40 +1816,40 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>9.4</v>
+        <v>6.2</v>
       </c>
       <c r="E28" t="n">
-        <v>1.800000000000001</v>
+        <v>1.7</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -9.5</t>
+          <t>San José State -1.5</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -7.5</t>
+          <t>San José State -1.5</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -9.3</t>
+          <t>Wyoming -0.2</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>9.300000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J28" t="n">
-        <v>7.5</v>
+        <v>-1.5</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
@@ -1866,40 +1866,40 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>9.199999999999999</v>
+        <v>5.4</v>
       </c>
       <c r="E29" t="n">
-        <v>1.800000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Texas Tech -14.0</t>
+          <t>UTSA -13.0</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Texas Tech -14.5</t>
+          <t>UTSA -13.0</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Texas Tech -12.7</t>
+          <t>UTSA -11.4</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>12.7</v>
+        <v>11.4</v>
       </c>
       <c r="J29" t="n">
-        <v>14.5</v>
+        <v>13</v>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Georgia -7.0</t>
+          <t>Georgia -3.5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1966,40 +1966,40 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>Michigan State</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3.1</v>
+        <v>7.1</v>
       </c>
       <c r="E31" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Miami (OH) -9.5</t>
+          <t>Michigan State -7.5</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Miami (OH) -10</t>
+          <t>Michigan State -9.0</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Miami (OH) -11.4</t>
+          <t>Michigan State -10.5</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>-11.4</v>
+        <v>10.5</v>
       </c>
       <c r="J31" t="n">
-        <v>-10</v>
+        <v>9</v>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
@@ -2016,40 +2016,40 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>9.9</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E32" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Oregon -14.5</t>
+          <t>Iowa State -5.0</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Oregon -7.5</t>
+          <t>Iowa State -3.0</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Oregon -6.2</t>
+          <t>Iowa State -4.5</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>6.2</v>
+        <v>-4.5</v>
       </c>
       <c r="J32" t="n">
-        <v>7.5</v>
+        <v>-3</v>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
@@ -2066,40 +2066,40 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>North Texas</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E33" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>North Texas -2.5</t>
+          <t>Navy -7.5</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>North Texas -1.5</t>
+          <t>Navy -9.5</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>North Texas -2.7</t>
+          <t>Navy -8.0</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>2.7</v>
+        <v>-8</v>
       </c>
       <c r="J33" t="n">
-        <v>1.5</v>
+        <v>-9.5</v>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
@@ -2116,40 +2116,40 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>3.7</v>
+        <v>6.3</v>
       </c>
       <c r="E34" t="n">
-        <v>1.100000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Ole Miss -32.5</t>
+          <t>Boise State -16.5</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Ole Miss -32.5</t>
+          <t>Boise State -16.0</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Ole Miss -33.6</t>
+          <t>Boise State -14.6</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>33.6</v>
+        <v>14.6</v>
       </c>
       <c r="J34" t="n">
-        <v>32.5</v>
+        <v>16</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
@@ -2166,40 +2166,40 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>5.7</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E35" t="n">
-        <v>1.100000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>SMU -18.5</t>
+          <t>Iowa -4.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>SMU -17.5</t>
+          <t>Iowa -3.0</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>SMU -18.6</t>
+          <t>Iowa -4.4</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>18.6</v>
+        <v>-4.4</v>
       </c>
       <c r="J35" t="n">
-        <v>17.5</v>
+        <v>-3</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
@@ -2216,40 +2216,40 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Troy</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9.800000000000001</v>
+        <v>6.7</v>
       </c>
       <c r="E36" t="n">
-        <v>1.1</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Michigan -1.5</t>
+          <t>Texas State -10.5</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>USC -1.5</t>
+          <t>Texas State -9.5</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>USC -2.6</t>
+          <t>Texas State -8.2</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>2.6</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="J36" t="n">
-        <v>1.5</v>
+        <v>9.5</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2266,40 +2266,40 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>4.5</v>
+        <v>9.9</v>
       </c>
       <c r="E37" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>App State -4.5</t>
+          <t>Oregon -9.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>App State -3</t>
+          <t>Oregon -7.5</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>App State -1.9</t>
+          <t>Oregon -6.2</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>-1.9</v>
+        <v>6.2</v>
       </c>
       <c r="J37" t="n">
-        <v>-3</v>
+        <v>7.5</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -2316,40 +2316,40 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>5.4</v>
+        <v>3.7</v>
       </c>
       <c r="E38" t="n">
-        <v>1.1</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>UTSA -10.5</t>
+          <t>Ole Miss -32.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>UTSA -12.5</t>
+          <t>Ole Miss -32.5</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>UTSA -11.4</t>
+          <t>Ole Miss -33.6</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>11.4</v>
+        <v>33.6</v>
       </c>
       <c r="J38" t="n">
-        <v>12.5</v>
+        <v>32.5</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2366,40 +2366,40 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>8.300000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="E39" t="n">
-        <v>0.9000000000000004</v>
+        <v>1.1</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Iowa -2.5</t>
+          <t>Cincinnati -10.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Iowa -3.5</t>
+          <t>Cincinnati -11.0</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Iowa -4.4</t>
+          <t>Cincinnati -9.9</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>-4.4</v>
+        <v>9.9</v>
       </c>
       <c r="J39" t="n">
-        <v>-3.5</v>
+        <v>11</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -2416,40 +2416,40 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>7.1</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E40" t="n">
-        <v>0.8999999999999986</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Penn State -21.5</t>
+          <t>Nebraska -5.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Penn State -21.5</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Penn State -20.6</t>
+          <t>Nebraska -5.6</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>20.6</v>
+        <v>-5.6</v>
       </c>
       <c r="J40" t="n">
-        <v>21.5</v>
+        <v>-6.5</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
@@ -2466,40 +2466,40 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Oklahoma State</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>4</v>
+        <v>7.7</v>
       </c>
       <c r="E41" t="n">
-        <v>0.8000000000000007</v>
+        <v>0.8999999999999986</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Houston -14.0</t>
+          <t>Notre Dame -22.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Houston -14</t>
+          <t>Notre Dame -21.5</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Houston -14.8</t>
+          <t>Notre Dame -22.4</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>-14.8</v>
+        <v>22.4</v>
       </c>
       <c r="J41" t="n">
-        <v>-14</v>
+        <v>21.5</v>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
@@ -2516,40 +2516,40 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>9.1</v>
+        <v>7.1</v>
       </c>
       <c r="E42" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.8999999999999986</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>LSU -10.5</t>
+          <t>Penn State -22.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>LSU -10</t>
+          <t>Penn State -21.5</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>LSU -10.7</t>
+          <t>Penn State -20.6</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>10.7</v>
+        <v>20.6</v>
       </c>
       <c r="J42" t="n">
-        <v>10</v>
+        <v>21.5</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2566,40 +2566,40 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>5</v>
+        <v>5.7</v>
       </c>
       <c r="E43" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.8999999999999986</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Old Dominion -12.5</t>
+          <t>SMU -18.0</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Old Dominion -14</t>
+          <t>SMU -19.5</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Old Dominion -13.3</t>
+          <t>SMU -18.6</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>-13.3</v>
+        <v>18.6</v>
       </c>
       <c r="J43" t="n">
-        <v>-14</v>
+        <v>19.5</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
@@ -2616,37 +2616,37 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>9</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E44" t="n">
-        <v>0.5999999999999996</v>
+        <v>0.8000000000000007</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Texas Tech -14.5</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Tennessee -13.5</t>
+          <t>Texas Tech -13.5</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Tennessee -12.9</t>
+          <t>Texas Tech -12.7</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>12.9</v>
+        <v>12.7</v>
       </c>
       <c r="J44" t="n">
         <v>13.5</v>
@@ -2666,40 +2666,40 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Oklahoma State</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>8.4</v>
+        <v>4</v>
       </c>
       <c r="E45" t="n">
-        <v>0.5999999999999996</v>
+        <v>0.8000000000000007</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Cincinnati -10.5</t>
+          <t>Houston -13.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Cincinnati -10.5</t>
+          <t>Houston -14.0</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cincinnati -9.9</t>
+          <t>Houston -14.8</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>9.9</v>
+        <v>-14.8</v>
       </c>
       <c r="J45" t="n">
-        <v>10.5</v>
+        <v>-14</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
@@ -2716,40 +2716,40 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>8.800000000000001</v>
+        <v>5.4</v>
       </c>
       <c r="E46" t="n">
-        <v>0.5</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Washington -10.0</t>
+          <t>Southern Miss -2.5</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Washington -10.5</t>
+          <t>Southern Miss -3.5</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Washington -10.0</t>
+          <t>Southern Miss -2.8</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>10</v>
+        <v>-2.8</v>
       </c>
       <c r="J46" t="n">
-        <v>10.5</v>
+        <v>-3.5</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
@@ -2766,40 +2766,40 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>8.300000000000001</v>
+        <v>5</v>
       </c>
       <c r="E47" t="n">
-        <v>0.5</v>
+        <v>0.6999999999999993</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Iowa State -4.5</t>
+          <t>Old Dominion -14.0</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Iowa State -4</t>
+          <t>Old Dominion -14.0</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Iowa State -4.5</t>
+          <t>Old Dominion -13.3</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>-4.5</v>
+        <v>-13.3</v>
       </c>
       <c r="J47" t="n">
-        <v>-4</v>
+        <v>-14</v>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
@@ -2816,40 +2816,40 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E48" t="n">
-        <v>0.5</v>
+        <v>0.6999999999999993</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Navy -9.5</t>
+          <t>Ohio State -14.5</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Navy -8.5</t>
+          <t>Ohio State -14.0</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Navy -8.0</t>
+          <t>Ohio State -13.3</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>-8</v>
+        <v>-13.3</v>
       </c>
       <c r="J48" t="n">
-        <v>-8.5</v>
+        <v>-14</v>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
@@ -2866,40 +2866,40 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>7.3</v>
+        <v>4.5</v>
       </c>
       <c r="E49" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Minnesota -10.5</t>
+          <t>App State -3.0</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Minnesota -9.5</t>
+          <t>App State -2.5</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Minnesota -9.9</t>
+          <t>App State -1.9</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>9.9</v>
+        <v>-1.9</v>
       </c>
       <c r="J49" t="n">
-        <v>9.5</v>
+        <v>-2.5</v>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
@@ -2916,40 +2916,40 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>7.1</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E50" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Georgia Tech -14.5</t>
+          <t>Washington -10.0</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Georgia Tech -14.5</t>
+          <t>Washington -10.5</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Georgia Tech -14.9</t>
+          <t>Washington -10.0</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>14.9</v>
+        <v>10</v>
       </c>
       <c r="J50" t="n">
-        <v>14.5</v>
+        <v>10.5</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
@@ -2966,40 +2966,40 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>8.800000000000001</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E51" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Nebraska -5.5</t>
+          <t>Alabama -4.0</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Nebraska -6</t>
+          <t>Alabama -3.0</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Nebraska -5.6</t>
+          <t>Alabama -3.5</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>-5.6</v>
+        <v>-3.5</v>
       </c>
       <c r="J51" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
@@ -3016,40 +3016,40 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>James Madison</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>4.8</v>
+        <v>9</v>
       </c>
       <c r="E52" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>James Madison -17.5</t>
+          <t>Tennessee -13.5</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>James Madison -17.5</t>
+          <t>Tennessee -12.5</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>James Madison -17.8</t>
+          <t>Tennessee -12.9</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>17.8</v>
+        <v>12.9</v>
       </c>
       <c r="J52" t="n">
-        <v>17.5</v>
+        <v>12.5</v>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
@@ -3066,40 +3066,40 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>5.4</v>
+        <v>3.1</v>
       </c>
       <c r="E53" t="n">
-        <v>0.2999999999999998</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Southern Miss -1.5</t>
+          <t>Miami (OH) -10.0</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Southern Miss -2.5</t>
+          <t>Miami (OH) -11.0</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Southern Miss -2.8</t>
+          <t>Miami (OH) -11.4</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>-2.8</v>
+        <v>-11.4</v>
       </c>
       <c r="J53" t="n">
-        <v>-2.5</v>
+        <v>-11</v>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
@@ -3132,12 +3132,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
+          <t>Kent State -2.5</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
           <t>Kent State -3.0</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Kent State -3</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -3166,40 +3166,40 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>James Madison</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>4.9</v>
+        <v>4.8</v>
       </c>
       <c r="E55" t="n">
-        <v>0.2000000000000002</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Liberty -3.0</t>
+          <t>James Madison -17.5</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Liberty -2.5</t>
+          <t>James Madison -18.0</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Liberty -2.7</t>
+          <t>James Madison -17.8</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>-2.7</v>
+        <v>17.8</v>
       </c>
       <c r="J55" t="n">
-        <v>-2.5</v>
+        <v>18</v>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
@@ -3216,40 +3216,40 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>7.7</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E56" t="n">
-        <v>0.1000000000000014</v>
+        <v>0.1000000000000001</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Notre Dame -21.5</t>
+          <t>USC -2.5</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Notre Dame -22.5</t>
+          <t>USC -2.5</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Notre Dame -22.4</t>
+          <t>USC -2.6</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>22.4</v>
+        <v>2.6</v>
       </c>
       <c r="J56" t="n">
-        <v>22.5</v>
+        <v>2.5</v>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
@@ -3266,40 +3266,40 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>9.699999999999999</v>
+        <v>7.1</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>0.09999999999999964</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Alabama -6.5</t>
+          <t>Georgia Tech -14.5</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Alabama -3.5</t>
+          <t>Georgia Tech -15.0</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Alabama -3.5</t>
+          <t>Georgia Tech -14.9</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>-3.5</v>
+        <v>14.9</v>
       </c>
       <c r="J57" t="n">
-        <v>-3.5</v>
+        <v>15</v>
       </c>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr"/>

</xml_diff>

<commit_message>
cleaning up some vegas spread things
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week7.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week7.xlsx
@@ -2316,40 +2316,40 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3.7</v>
+        <v>5</v>
       </c>
       <c r="E38" t="n">
-        <v>1.100000000000001</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Ole Miss -32.5</t>
+          <t>Old Dominion -14.0</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Ole Miss -32.5</t>
+          <t>Old Dominion -14.5</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Ole Miss -33.6</t>
+          <t>Old Dominion -13.3</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>33.6</v>
+        <v>-13.3</v>
       </c>
       <c r="J38" t="n">
-        <v>32.5</v>
+        <v>-14.5</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2366,40 +2366,40 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>8.4</v>
+        <v>3.7</v>
       </c>
       <c r="E39" t="n">
-        <v>1.1</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Cincinnati -10.5</t>
+          <t>Ole Miss -32.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Cincinnati -11.0</t>
+          <t>Ole Miss -32.5</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Cincinnati -9.9</t>
+          <t>Ole Miss -33.6</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>9.9</v>
+        <v>33.6</v>
       </c>
       <c r="J39" t="n">
-        <v>11</v>
+        <v>32.5</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -2416,40 +2416,40 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>8.800000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="E40" t="n">
-        <v>0.9000000000000004</v>
+        <v>1.1</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Nebraska -5.5</t>
+          <t>Cincinnati -10.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>Cincinnati -11.0</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Nebraska -5.6</t>
+          <t>Cincinnati -9.9</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>-5.6</v>
+        <v>9.9</v>
       </c>
       <c r="J40" t="n">
-        <v>-6.5</v>
+        <v>11</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
@@ -2466,40 +2466,40 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>7.7</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E41" t="n">
-        <v>0.8999999999999986</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Notre Dame -22.5</t>
+          <t>Nebraska -5.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Notre Dame -21.5</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Notre Dame -22.4</t>
+          <t>Nebraska -5.6</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>22.4</v>
+        <v>-5.6</v>
       </c>
       <c r="J41" t="n">
-        <v>21.5</v>
+        <v>-6.5</v>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
@@ -2516,37 +2516,37 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>7.1</v>
+        <v>7.7</v>
       </c>
       <c r="E42" t="n">
         <v>0.8999999999999986</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Penn State -22.5</t>
+          <t>Notre Dame -22.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Penn State -21.5</t>
+          <t>Notre Dame -21.5</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Penn State -20.6</t>
+          <t>Notre Dame -22.4</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>20.6</v>
+        <v>22.4</v>
       </c>
       <c r="J42" t="n">
         <v>21.5</v>
@@ -2566,40 +2566,40 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>5.7</v>
+        <v>7.1</v>
       </c>
       <c r="E43" t="n">
         <v>0.8999999999999986</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>SMU -18.0</t>
+          <t>Penn State -22.5</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>SMU -19.5</t>
+          <t>Penn State -21.5</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>SMU -18.6</t>
+          <t>Penn State -20.6</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>18.6</v>
+        <v>20.6</v>
       </c>
       <c r="J43" t="n">
-        <v>19.5</v>
+        <v>21.5</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
@@ -2616,40 +2616,40 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>9.199999999999999</v>
+        <v>5.7</v>
       </c>
       <c r="E44" t="n">
-        <v>0.8000000000000007</v>
+        <v>0.8999999999999986</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Texas Tech -14.5</t>
+          <t>SMU -18.0</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Texas Tech -13.5</t>
+          <t>SMU -19.5</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Texas Tech -12.7</t>
+          <t>SMU -18.6</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>12.7</v>
+        <v>18.6</v>
       </c>
       <c r="J44" t="n">
-        <v>13.5</v>
+        <v>19.5</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -2666,40 +2666,40 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Oklahoma State</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>4</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E45" t="n">
         <v>0.8000000000000007</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Houston -13.5</t>
+          <t>Texas Tech -14.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Houston -14.0</t>
+          <t>Texas Tech -13.5</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Houston -14.8</t>
+          <t>Texas Tech -12.7</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>-14.8</v>
+        <v>12.7</v>
       </c>
       <c r="J45" t="n">
-        <v>-14</v>
+        <v>13.5</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
@@ -2716,40 +2716,40 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Oklahoma State</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>5.4</v>
+        <v>4</v>
       </c>
       <c r="E46" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.8000000000000007</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Southern Miss -2.5</t>
+          <t>Houston -13.5</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Southern Miss -3.5</t>
+          <t>Houston -14.0</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Southern Miss -2.8</t>
+          <t>Houston -14.8</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>-2.8</v>
+        <v>-14.8</v>
       </c>
       <c r="J46" t="n">
-        <v>-3.5</v>
+        <v>-14</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
@@ -2766,40 +2766,40 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>5</v>
+        <v>5.4</v>
       </c>
       <c r="E47" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Old Dominion -14.0</t>
+          <t>Southern Miss -2.5</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Old Dominion -14.0</t>
+          <t>Southern Miss -3.5</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Old Dominion -13.3</t>
+          <t>Southern Miss -2.8</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>-13.3</v>
+        <v>-2.8</v>
       </c>
       <c r="J47" t="n">
-        <v>-14</v>
+        <v>-3.5</v>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>

</xml_diff>